<commit_message>
subtask 1 + outliers
subtask 1 + outliers
</commit_message>
<xml_diff>
--- a/projects/maintenance_industry_4_2024/dataset/training_data/Test conditions.xlsx
+++ b/projects/maintenance_industry_4_2024/dataset/training_data/Test conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centralesupelec-my.sharepoint.com/personal/zhiguo_zeng_centralesupelec_fr/Documents/Code/Python/digital_twin_robot/robot_digital_twin/condition_monitoring_matlab_ros/matlab_application/collected_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_F25DC773A252ABDACC1048B9511F42AE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90877791-9C7E-4912-B110-4EF4C774E5E5}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_F25DC773A252ABDACC1048B9511F42AE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED028A56-8B9A-45A0-BAB4-D2A98AEC96AF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Test id</t>
   </si>
@@ -82,42 +82,6 @@
   </si>
   <si>
     <t>Starting position: Straigt. Perform two operations</t>
-  </si>
-  <si>
-    <t>20240425_093699</t>
-  </si>
-  <si>
-    <t>Not moving</t>
-  </si>
-  <si>
-    <t>20240425_094425</t>
-  </si>
-  <si>
-    <t>20240426_141190</t>
-  </si>
-  <si>
-    <t>Pick up a box from the shelf and move it to another shelf</t>
-  </si>
-  <si>
-    <t>20240426_140055</t>
-  </si>
-  <si>
-    <t>20240426_141532</t>
-  </si>
-  <si>
-    <t>Moving one motor</t>
-  </si>
-  <si>
-    <t>20240426_141602</t>
-  </si>
-  <si>
-    <t>20240426_141726</t>
-  </si>
-  <si>
-    <t>20240426_141938</t>
-  </si>
-  <si>
-    <t>20240426_141980</t>
   </si>
 </sst>
 </file>
@@ -435,19 +399,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -463,7 +427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -471,7 +435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -479,7 +443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -487,7 +451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -495,7 +459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -503,7 +467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -511,7 +475,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -519,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -527,84 +491,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more test on motor 6
</commit_message>
<xml_diff>
--- a/projects/maintenance_industry_4_2024/dataset/training_data/Test conditions.xlsx
+++ b/projects/maintenance_industry_4_2024/dataset/training_data/Test conditions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centralesupelec-my.sharepoint.com/personal/zhiguo_zeng_centralesupelec_fr/Documents/Code/Python/digital_twin_robot/projects/maintenance_industry_4_2024/dataset/training_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centralesupelec-my.sharepoint.com/personal/zhiguo_zeng_centralesupelec_fr/Documents/Code/Python/digital_twin_robot/robot_digital_twin/condition_monitoring_matlab_ros/matlab_application/collected_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC1048B9511F42AE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5087CF59-21AD-4156-A03D-E02E57D4319E}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC1048B9511F42AE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBDABE11-6EED-4BA3-8E55-F1208B668B34}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Test id</t>
   </si>
@@ -36,42 +36,24 @@
     <t>20240105_164214</t>
   </si>
   <si>
-    <t>Robot not moving, just starting up.</t>
-  </si>
-  <si>
     <t>20240105_165300</t>
   </si>
   <si>
-    <t>Not moving. Then perform a pick-up and place operation.</t>
-  </si>
-  <si>
     <t>20240105_165972</t>
   </si>
   <si>
-    <t>Not moving. After the operation.</t>
-  </si>
-  <si>
     <t>20240320_152031</t>
   </si>
   <si>
     <t>20240320_153841</t>
   </si>
   <si>
-    <t>Not moving. Move motor 6 -&gt; motor 1 sequentially.</t>
-  </si>
-  <si>
     <t>20240320_155664</t>
   </si>
   <si>
-    <t>Robot not moving.</t>
-  </si>
-  <si>
     <t>20240321_122650</t>
   </si>
   <si>
-    <t>Try to move to pick up an item from second floor of a shelf. But failed.</t>
-  </si>
-  <si>
     <t>20240325_135213</t>
   </si>
   <si>
@@ -81,9 +63,6 @@
     <t>20240325_155003</t>
   </si>
   <si>
-    <t>Starting position: Straigt. Perform two operations</t>
-  </si>
-  <si>
     <t>20240425_093699</t>
   </si>
   <si>
@@ -96,9 +75,6 @@
     <t>20240426_141190</t>
   </si>
   <si>
-    <t>Pick up a box from the shelf and move it to another shelf</t>
-  </si>
-  <si>
     <t>20240426_140055</t>
   </si>
   <si>
@@ -136,6 +112,27 @@
   </si>
   <si>
     <t>Motor_6_failure</t>
+  </si>
+  <si>
+    <t>20240503_163963</t>
+  </si>
+  <si>
+    <t>20240503_164435</t>
+  </si>
+  <si>
+    <t>Turning motor 6</t>
+  </si>
+  <si>
+    <t>20240503_164675</t>
+  </si>
+  <si>
+    <t>20240503_165189</t>
+  </si>
+  <si>
+    <t>Pick up and place</t>
+  </si>
+  <si>
+    <t>Move motor 6 -&gt; motor 1 sequentially.</t>
   </si>
 </sst>
 </file>
@@ -453,20 +450,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,216 +471,257 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
-        <v>26</v>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>